<commit_message>
01 mai 2016 apres long temp
</commit_message>
<xml_diff>
--- a/casedata_ex.xlsx
+++ b/casedata_ex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="casedata_ex" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>arbaminch</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>a= 0, b=6, c=2</t>
+  </si>
+  <si>
+    <t>attr4</t>
+  </si>
+  <si>
+    <t>yesnotest</t>
+  </si>
+  <si>
+    <t>drange</t>
+  </si>
+  <si>
+    <t>lower=0, upper=1</t>
   </si>
 </sst>
 </file>
@@ -97,7 +109,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,7 +125,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFEBF6"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFBFEBF6"/>
       </patternFill>
     </fill>
   </fills>
@@ -151,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,15 +182,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,7 +246,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -253,17 +279,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.6530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,21 +313,21 @@
         <v>121000</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" s="3" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+    <row r="5" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+    <row r="6" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -309,36 +335,56 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" s="3" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+    <row r="11" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5" t="s">
+    <row r="12" s="5" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>